<commit_message>
Change hearingType to type
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/interim-applications-chd-daily-cause-list/interimApplicationsChanceryDivisionDailyCauseList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/interim-applications-chd-daily-cause-list/interimApplicationsChanceryDivisionDailyCauseList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natasha.alker/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914A4D75-6427-CB41-8771-7995E0930608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA4AD49-5D41-444D-8FD5-8238374F518D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16140" windowHeight="19500" activeTab="1" xr2:uid="{9A364F00-DA1E-184E-8EC3-0A8142389C9B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16140" windowHeight="19500" xr2:uid="{9A364F00-DA1E-184E-8EC3-0A8142389C9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hearing List" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>Name to be Displayed</t>
   </si>
   <si>
-    <t>Hearing Type</t>
-  </si>
-  <si>
     <t>Judge A</t>
   </si>
   <si>
@@ -75,12 +72,6 @@
     <t>This is a venue name</t>
   </si>
   <si>
-    <t>Case type A</t>
-  </si>
-  <si>
-    <t>Case type B</t>
-  </si>
-  <si>
     <t>This is a case name</t>
   </si>
   <si>
@@ -90,13 +81,22 @@
     <t>Judge C</t>
   </si>
   <si>
-    <t>Case type C</t>
-  </si>
-  <si>
     <t>Judge OpenJusticeTest</t>
   </si>
   <si>
     <t>judge.openjusticetest@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Type A</t>
+  </si>
+  <si>
+    <t>Type B</t>
+  </si>
+  <si>
+    <t>Type C</t>
   </si>
 </sst>
 </file>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9BC5ED-E237-584F-BFE6-7D785EA2CF3D}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,7 +516,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -530,71 +530,71 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3">
         <v>0.4375</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>1234</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>0.4375</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>3456</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3">
         <v>0.4375</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>5678</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -606,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA013B87-7606-2045-B713-A9C1666DEACC}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -626,10 +626,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>